<commit_message>
CAN1-64 Tx Priority Testcases Revision
Revised testcases based on requirements CR - Devon
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/tx_priority_testcases.xlsx
+++ b/Documentations/Test Cases/tx_priority_testcases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djste\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djste\Documents\GitHub\CAN_we_do_it_Can_Controller\Documentations\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE47F21D-FE6A-41E7-B952-0D6C602D9D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2538CC9E-F80D-4FA5-B241-8AE018DE4BB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D9DD170-8ED8-4417-B493-FE566D307589}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="100">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -179,30 +179,12 @@
     <t>‘o_send_data’[127:0], ‘o_send_en’, ‘o_hpb_r_en’ and ‘o_fifo_r_en’ outputs shall be set to zeros when ‘i_reset’ is set to 1.</t>
   </si>
   <si>
-    <t>The state shall transition from send_fifo to idle when ‘i_busy_can’ is set to 1 and ‘i_cen’ is set to 1.</t>
-  </si>
-  <si>
-    <t>The state shall transition from send_hpb to idle when ‘i_busy_can’ is set to 1 and ‘i_cen’ is set to 1.</t>
-  </si>
-  <si>
-    <t>‘o_send_data’[127:0] shall be set to the latched data when the state is in send_hpb or send_fifo.</t>
-  </si>
-  <si>
-    <t>‘o_send_en’ shall be set to 1 when the state is in send_hpb or send_fifo.</t>
-  </si>
-  <si>
-    <t>‘i_fifo_data’[127:0] shall be latched internally when the state transitions from prepare to send_fifo.</t>
-  </si>
-  <si>
     <t>‘o_fifo_r_en’ shall be pulsed for one system clock cycle when the state transitions from prepare to send_fifo.</t>
   </si>
   <si>
     <t>The state shall transition from prepare to send_fifo when ‘i_busy_can’ is set to 0, ‘i_cen’ is set to 1, ‘i_hpbfull’ is set to 0 and ‘i_tx_empty’ is set to 0.</t>
   </si>
   <si>
-    <t>‘i_hpb_data’[127:0] shall be latched internally when the state transitions from prepare to send_hpb.</t>
-  </si>
-  <si>
     <t>‘o_hpb_r_en’ shall be pulsed for one system clock cycle when the state transitions from prepare to send_hpb.</t>
   </si>
   <si>
@@ -210,6 +192,117 @@
   </si>
   <si>
     <t>The state shall transition from idle to prepare when ‘i_busy_can’ is set to 0 and ‘i_cen’ is set to 1.</t>
+  </si>
+  <si>
+    <t>i_reset' = 1</t>
+  </si>
+  <si>
+    <t>o_send_data'[127:0] = 128b'0
+'o_send_en' = 0
+'o_hpb_r_en' = 0
+'o_fifo_r_en' = 0</t>
+  </si>
+  <si>
+    <t>Initialize 100Mhz system clock
+Initialize 25Mhz CAN clock
+Instantiate module
+set 'i_reset' to 1</t>
+  </si>
+  <si>
+    <t>o_send_en' = 0</t>
+  </si>
+  <si>
+    <t>i_busy_can' = 0
+'i_cen' = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set 'i_hpbfull' to 1
+</t>
+  </si>
+  <si>
+    <t>i_hpbfull' = 1</t>
+  </si>
+  <si>
+    <t>check current state is send_hpb</t>
+  </si>
+  <si>
+    <t>o_hpb_r_en' = 1 for one system clock cycle</t>
+  </si>
+  <si>
+    <t>i_busy_can' = 0
+'i_cen' = 1
+i_tx_empty  = 0</t>
+  </si>
+  <si>
+    <t>check current state is send_fifo</t>
+  </si>
+  <si>
+    <t>o_fifo_r_en' = 1 for one system clock</t>
+  </si>
+  <si>
+    <t>o_send_en' = 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set 'i_busy_can' to 1
+</t>
+  </si>
+  <si>
+    <t>Observation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set 'i_busy_can' to 0
+set 'i_cen' to 1
+</t>
+  </si>
+  <si>
+    <t>instantiate module for testing send_hpb state
+check initial system state
+set 'i_reset' to 1
+set 'i_tx_empty' = 1
+check state is in idle
+observe 'o_send_en'</t>
+  </si>
+  <si>
+    <t>TXPL_20</t>
+  </si>
+  <si>
+    <t>The state shall transition from send_fifo to send after one clock cycle.</t>
+  </si>
+  <si>
+    <t>‘o_send_data’[127:0] shall be synchronized to ‘i_can_clk’.</t>
+  </si>
+  <si>
+    <t>‘o_send_en’ shall be synchronized to ‘i_can_clk’.</t>
+  </si>
+  <si>
+    <t>‘i_busy_can’ shall be synchronized to ‘i_sys_clk’.</t>
+  </si>
+  <si>
+    <t>All state transitions and signal manipulation shall occur using ‘i_sys_clk’.</t>
+  </si>
+  <si>
+    <t>The implemented state machine shall have at least the following states: idle, prepare, send_hpb, send_fifo and send.</t>
+  </si>
+  <si>
+    <t>‘state’ shall be initialized at idle state.</t>
+  </si>
+  <si>
+    <t>‘state’ shall transition to and stay in idle state when ‘i_reset’ is set to 1.</t>
+  </si>
+  <si>
+    <t>‘o_send_en’ shall be set to 0 in all states except in send state.</t>
+  </si>
+  <si>
+    <t>‘i_hpb_data’[127:0] shall be latched internally in ‘latch_data’[127:0] when the state transitions from prepare to send_hpb.</t>
+  </si>
+  <si>
+    <t>The state shall transition from send_hpb to send after one clock cycle.</t>
+  </si>
+  <si>
+    <t>‘i_fifo_data’[127:0] shall be latched internally to ‘latch_data’[127:0] when the state transitions from prepare to send_fifo.</t>
+  </si>
+  <si>
+    <t>‘o_send_en’ shall be set to 1 when the state is in send.</t>
   </si>
   <si>
     <r>
@@ -229,124 +322,59 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>‘o_send_en’ shall be set to 0 when the state is in idle.</t>
+      <t>‘o_send_data’[127:0] shall be set to the latched data when the state is in send.</t>
     </r>
   </si>
   <si>
-    <t>The state machine shall transition to and stay in idle state when ‘i_reset’ is set to 1.</t>
-  </si>
-  <si>
-    <t>The state machine shall be initialized at idle state.</t>
-  </si>
-  <si>
-    <t>The implemented state machine shall have at least the following states: idle, prepare, send_hpb and send_fifo.</t>
-  </si>
-  <si>
-    <t>‘i_busy_can’ shall be synchronized to the system clock.</t>
-  </si>
-  <si>
-    <t>‘o_send_en’ shall be synchronized to the CAN clock.</t>
-  </si>
-  <si>
-    <t>‘o_send_data’[127:0] shall be synchronized to the CAN clock.</t>
-  </si>
-  <si>
-    <t>i_reset' = 1</t>
-  </si>
-  <si>
-    <t>o_send_data'[127:0] = 128b'0
-'o_send_en' = 0
-'o_hpb_r_en' = 0
-'o_fifo_r_en' = 0</t>
-  </si>
-  <si>
-    <t>current_state = idle</t>
-  </si>
-  <si>
-    <t>Initialize 100Mhz system clock
-Initialize 25Mhz CAN clock
-Instantiate module
-set 'i_reset' to 1</t>
-  </si>
-  <si>
-    <t>o_send_en' = 0</t>
-  </si>
-  <si>
-    <t>i_busy_can' = 0
+    <t>The state shall transition from send to prepare when ‘i_busy_can’ is set to 1 and ‘i_cen’ is set to 1.</t>
+  </si>
+  <si>
+    <t>TXPL_TC_20</t>
+  </si>
+  <si>
+    <t>TXPL_TC_21</t>
+  </si>
+  <si>
+    <t>TXPL_21</t>
+  </si>
+  <si>
+    <t>state' = idle</t>
+  </si>
+  <si>
+    <t>state' = prepare</t>
+  </si>
+  <si>
+    <t>state' = send_hpb</t>
+  </si>
+  <si>
+    <t>latch_data' = 'i_hpb_data'[127:0]</t>
+  </si>
+  <si>
+    <t>state' = send after one clock cycle</t>
+  </si>
+  <si>
+    <t>state' = send_fifo</t>
+  </si>
+  <si>
+    <t>check current state is send</t>
+  </si>
+  <si>
+    <t>o_send_data' = 'latch_data'</t>
+  </si>
+  <si>
+    <t>latch_data' = 'i_fifo_data'[127:0]</t>
+  </si>
+  <si>
+    <t>i_busy_can' = 1
 'i_cen' = 1</t>
   </si>
   <si>
-    <t>current_state = prepare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set 'i_hpbfull' to 1
-</t>
-  </si>
-  <si>
-    <t>i_hpbfull' = 1</t>
-  </si>
-  <si>
-    <t>current_state = send_hpb</t>
-  </si>
-  <si>
-    <t>check current state is send_hpb</t>
-  </si>
-  <si>
-    <t>o_hpb_r_en' = 1 for one system clock cycle</t>
-  </si>
-  <si>
-    <t>current_state = send_fifo</t>
-  </si>
-  <si>
-    <t>i_busy_can' = 0
-'i_cen' = 1
-i_tx_empty  = 0</t>
-  </si>
-  <si>
-    <t>check current state is send_fifo</t>
-  </si>
-  <si>
-    <t>o_fifo_r_en' = 1 for one system clock</t>
-  </si>
-  <si>
-    <t>o_send_en' = 1</t>
-  </si>
-  <si>
-    <t>o_send_en' = fifo_latch</t>
-  </si>
-  <si>
-    <t>fifo_latch = 'i_fifo_data'[127:0]</t>
-  </si>
-  <si>
-    <t>hpb_latch = 'i_hpb_data'[127:0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set 'i_busy_can' to 1
-</t>
-  </si>
-  <si>
-    <t>Observation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set 'i_busy_can' to 0
-set 'i_cen' to 1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">instantiate new module for testing send_fifo state
+    <t xml:space="preserve">instantiate new module for testing send_fifo and send state
 set 'i_busy_can' to 0
 set 'i_cen' to 1
 check current state is prepare
 set 'i_tx_empty' to 0
 </t>
-  </si>
-  <si>
-    <t>instantiate module for testing send_hpb state
-check initial system state
-set 'i_reset' to 1
-set 'i_tx_empty' = 1
-check state is in idle
-observe 'o_send_en'</t>
   </si>
 </sst>
 </file>
@@ -409,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -418,15 +446,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -436,6 +460,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,18 +784,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73642E39-ECFF-4314-AFC1-488407319D91}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.28515625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" customWidth="1"/>
+    <col min="3" max="3" width="47.5703125" customWidth="1"/>
+    <col min="4" max="4" width="62.42578125" customWidth="1"/>
     <col min="5" max="5" width="31" customWidth="1"/>
     <col min="6" max="6" width="47.140625" customWidth="1"/>
     <col min="7" max="7" width="34.85546875" customWidth="1"/>
@@ -799,24 +832,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>67</v>
+      <c r="D2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -827,13 +860,17 @@
         <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -841,13 +878,13 @@
         <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -855,13 +892,13 @@
         <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -869,13 +906,13 @@
         <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -883,16 +920,13 @@
         <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -900,32 +934,35 @@
         <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="F9" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -933,16 +970,12 @@
         <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" t="s">
-        <v>72</v>
+        <v>79</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -953,19 +986,19 @@
         <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="F11" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -973,16 +1006,19 @@
         <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -990,113 +1026,123 @@
         <v>39</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="F13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B19" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="F17" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="F18" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="F19" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="9"/>
+      <c r="F19" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1104,20 +1150,58 @@
         <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
         <v>86</v>
       </c>
-      <c r="F20" t="s">
-        <v>68</v>
+      <c r="C21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D16:D19"/>
+  <mergeCells count="6">
+    <mergeCell ref="F3:F7"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D19:D21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CAN1-64 update tx priority testcases
updated requested changes - Devon
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/tx_priority_testcases.xlsx
+++ b/Documentations/Test Cases/tx_priority_testcases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djste\Documents\GitHub\CAN_we_do_it_Can_Controller\Documentations\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2538CC9E-F80D-4FA5-B241-8AE018DE4BB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F973FE9D-7421-4ED4-817D-A6114418613F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D9DD170-8ED8-4417-B493-FE566D307589}"/>
+    <workbookView xWindow="11010" yWindow="0" windowWidth="15795" windowHeight="11385" xr2:uid="{6D9DD170-8ED8-4417-B493-FE566D307589}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,18 +220,10 @@
 </t>
   </si>
   <si>
-    <t>i_hpbfull' = 1</t>
-  </si>
-  <si>
     <t>check current state is send_hpb</t>
   </si>
   <si>
     <t>o_hpb_r_en' = 1 for one system clock cycle</t>
-  </si>
-  <si>
-    <t>i_busy_can' = 0
-'i_cen' = 1
-i_tx_empty  = 0</t>
   </si>
   <si>
     <t>check current state is send_fifo</t>
@@ -248,11 +240,6 @@
   </si>
   <si>
     <t>Observation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set 'i_busy_can' to 0
-set 'i_cen' to 1
-</t>
   </si>
   <si>
     <t>instantiate module for testing send_hpb state
@@ -375,6 +362,22 @@
 check current state is prepare
 set 'i_tx_empty' to 0
 </t>
+  </si>
+  <si>
+    <t>set 'i_reset' to 0
+set 'i_busy_can' to 0
+set 'i_cen' to 1</t>
+  </si>
+  <si>
+    <t>i_busy_can' = 0
+'i_cen' = 1
+'i_hpbfull' = 1</t>
+  </si>
+  <si>
+    <t>i_busy_can' = 0
+'i_cen' = 1
+'i_tx_empty'  = 0
+'i_hpbfull' = 0</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -456,12 +459,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -469,6 +466,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73642E39-ECFF-4314-AFC1-488407319D91}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,10 +851,10 @@
       <c r="D2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="8" t="s">
         <v>54</v>
       </c>
     </row>
@@ -860,14 +866,14 @@
         <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="10" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -878,11 +884,11 @@
         <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="8"/>
+        <v>70</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="10"/>
     </row>
     <row r="5" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -892,11 +898,11 @@
         <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="10"/>
     </row>
     <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -906,11 +912,11 @@
         <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8"/>
+        <v>72</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="10"/>
     </row>
     <row r="7" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -920,11 +926,11 @@
         <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="8"/>
+        <v>73</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -934,14 +940,14 @@
         <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="11" t="s">
-        <v>89</v>
+        <v>74</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
@@ -952,14 +958,14 @@
         <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>89</v>
+      <c r="F9" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -970,15 +976,15 @@
         <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -988,14 +994,14 @@
       <c r="C11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="D11" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>90</v>
+      <c r="F11" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1011,11 +1017,11 @@
       <c r="D12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>91</v>
+      <c r="E12" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="57" customHeight="1" x14ac:dyDescent="0.25">
@@ -1028,12 +1034,12 @@
       <c r="C13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="11" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1044,12 +1050,12 @@
         <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="11" t="s">
-        <v>92</v>
+        <v>77</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1060,14 +1066,14 @@
         <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E15" s="9"/>
-      <c r="F15" s="11" t="s">
-        <v>93</v>
+        <v>64</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
@@ -1081,13 +1087,13 @@
         <v>49</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>94</v>
+      <c r="F16" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1100,12 +1106,12 @@
       <c r="C17" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="11" t="s">
-        <v>64</v>
+      <c r="D17" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="9" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1116,12 +1122,12 @@
         <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="11" t="s">
-        <v>97</v>
+        <v>79</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1132,14 +1138,14 @@
         <v>45</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="11" t="s">
-        <v>93</v>
+        <v>68</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1150,58 +1156,58 @@
         <v>46</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="11" t="s">
-        <v>65</v>
+        <v>80</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="11" t="s">
-        <v>96</v>
+        <v>81</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D19:D21"/>
     <mergeCell ref="F3:F7"/>
     <mergeCell ref="D3:D7"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D17:D18"/>
-    <mergeCell ref="D19:D21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>